<commit_message>
Add transactions.xlsx with transaction_id, product_id, price
</commit_message>
<xml_diff>
--- a/Projects/openpyxl/transactions.xlsx
+++ b/Projects/openpyxl/transactions.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,10 +29,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>product_id</t>
+    <t>transaction_id</t>
   </si>
   <si>
-    <t>transaction_id</t>
+    <t>product_id</t>
   </si>
   <si>
     <t>price</t>
@@ -376,7 +376,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="118" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -386,10 +386,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -420,6 +420,7 @@
       <c r="C3" s="3">
         <v>6.95</v>
       </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -431,6 +432,7 @@
       <c r="C4" s="3">
         <v>7.95</v>
       </c>
+      <c r="D4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>